<commit_message>
updated readme with screenshots
</commit_message>
<xml_diff>
--- a/July 2020 Rentals/BLM Rents July 2020.xlsx
+++ b/July 2020 Rentals/BLM Rents July 2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="42280" yWindow="3840" windowWidth="30760" windowHeight="17280"/>
+    <workbookView xWindow="39920" yWindow="3580" windowWidth="35680" windowHeight="20220"/>
   </bookViews>
   <sheets>
     <sheet name="R&amp;R" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="94">
   <si>
     <t xml:space="preserve">R &amp; R ROYALTY </t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>Maybe Let Go: No new produciton activity wihtin last 4 years near lease.  Latest lease taken within 2 mile raidus was in 2/20 for 26/acre by san juan properties.  Our comments say we gave 10% WI to Espejo - blm records do not show this transfer</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -651,7 +654,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -744,9 +747,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="34" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="34" applyFont="1"/>
@@ -858,6 +858,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1260,7 +1269,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1273,47 +1282,47 @@
     <col min="6" max="6" width="16.1640625" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="8" max="8" width="22.5" customWidth="1"/>
-    <col min="9" max="9" width="36.6640625" style="100" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" style="99" customWidth="1"/>
     <col min="10" max="10" width="14.5" customWidth="1"/>
     <col min="11" max="11" width="20.83203125" customWidth="1"/>
     <col min="12" max="12" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
     </row>
     <row r="2" spans="1:11" ht="20">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
     </row>
     <row r="3" spans="1:11" ht="15">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1"/>
@@ -1360,12 +1369,12 @@
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="100" t="s">
+      <c r="I5" s="99" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="87" t="s">
         <v>68</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -1374,27 +1383,29 @@
       <c r="C6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="89">
         <v>47300</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="67">
         <v>40</v>
       </c>
-      <c r="F6" s="72">
+      <c r="F6" s="71">
         <v>60</v>
       </c>
       <c r="G6" s="24"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="109" t="s">
+      <c r="H6" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="98" t="s">
+      <c r="J6" s="97" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="98"/>
+      <c r="K6" s="97"/>
     </row>
     <row r="7" spans="1:11" s="12" customFormat="1">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="87" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -1403,18 +1414,20 @@
       <c r="C7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="90">
+      <c r="D7" s="89">
         <v>47300</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="67">
         <v>80</v>
       </c>
-      <c r="F7" s="72">
+      <c r="F7" s="71">
         <v>120</v>
       </c>
       <c r="G7" s="24"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="109" t="s">
+      <c r="H7" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J7" s="13" t="s">
@@ -1426,7 +1439,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="5" customFormat="1">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="87" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -1435,21 +1448,23 @@
       <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="90">
+      <c r="D8" s="89">
         <v>47300</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="67">
         <v>430.5</v>
       </c>
-      <c r="F8" s="72">
+      <c r="F8" s="71">
         <v>646.5</v>
       </c>
       <c r="G8" s="24">
         <f>SUM(F6:F8)</f>
         <v>826.5</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="109" t="s">
+      <c r="H8" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J8" s="13" t="s">
@@ -1460,16 +1475,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="80" customFormat="1">
-      <c r="A9" s="88"/>
+    <row r="9" spans="1:11" s="79" customFormat="1">
+      <c r="A9" s="87"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="72"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
       <c r="G9" s="24"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="101"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="100"/>
       <c r="J9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1478,8 +1493,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="80" customFormat="1">
-      <c r="A10" s="88" t="s">
+    <row r="10" spans="1:11" s="79" customFormat="1">
+      <c r="A10" s="87" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -1488,18 +1503,20 @@
       <c r="C10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="90">
+      <c r="D10" s="89">
         <v>47300</v>
       </c>
-      <c r="E10" s="71">
+      <c r="E10" s="70">
         <v>160</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="71">
         <v>240</v>
       </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="109" t="s">
+      <c r="H10" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J10" s="13" t="s">
@@ -1510,8 +1527,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="80" customFormat="1">
-      <c r="A11" s="88" t="s">
+    <row r="11" spans="1:11" s="79" customFormat="1">
+      <c r="A11" s="87" t="s">
         <v>73</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -1520,18 +1537,20 @@
       <c r="C11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="90">
+      <c r="D11" s="89">
         <v>47300</v>
       </c>
-      <c r="E11" s="71">
+      <c r="E11" s="70">
         <v>480</v>
       </c>
-      <c r="F11" s="72">
+      <c r="F11" s="71">
         <v>720</v>
       </c>
       <c r="G11" s="24"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="109" t="s">
+      <c r="H11" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J11" s="13" t="s">
@@ -1542,8 +1561,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="80" customFormat="1">
-      <c r="A12" s="88" t="s">
+    <row r="12" spans="1:11" s="79" customFormat="1">
+      <c r="A12" s="87" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -1552,21 +1571,23 @@
       <c r="C12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="90">
+      <c r="D12" s="89">
         <v>47300</v>
       </c>
-      <c r="E12" s="71">
+      <c r="E12" s="70">
         <v>2080</v>
       </c>
-      <c r="F12" s="72">
+      <c r="F12" s="71">
         <v>3120</v>
       </c>
       <c r="G12" s="24">
         <f>SUM(F10:F12)</f>
         <v>4080</v>
       </c>
-      <c r="H12" s="74"/>
-      <c r="I12" s="109" t="s">
+      <c r="H12" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J12" s="13" t="s">
@@ -1577,16 +1598,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="80" customFormat="1">
-      <c r="A13" s="88"/>
+    <row r="13" spans="1:11" s="79" customFormat="1">
+      <c r="A13" s="87"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="72"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="71"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="101"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="100"/>
       <c r="J13" s="13" t="s">
         <v>22</v>
       </c>
@@ -1595,8 +1616,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="80" customFormat="1">
-      <c r="A14" s="88" t="s">
+    <row r="14" spans="1:11" s="79" customFormat="1">
+      <c r="A14" s="87" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="16" t="s">
@@ -1605,18 +1626,20 @@
       <c r="C14" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="90">
+      <c r="D14" s="89">
         <v>47300</v>
       </c>
-      <c r="E14" s="71">
+      <c r="E14" s="70">
         <v>338.59</v>
       </c>
-      <c r="F14" s="72">
+      <c r="F14" s="71">
         <v>508.5</v>
       </c>
       <c r="G14" s="24"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="109" t="s">
+      <c r="H14" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J14" s="13" t="s">
@@ -1627,8 +1650,8 @@
         <v>9472.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="80" customFormat="1">
-      <c r="A15" s="88" t="s">
+    <row r="15" spans="1:11" s="79" customFormat="1">
+      <c r="A15" s="87" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="16" t="s">
@@ -1637,18 +1660,20 @@
       <c r="C15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="90">
+      <c r="D15" s="89">
         <v>47300</v>
       </c>
-      <c r="E15" s="71">
+      <c r="E15" s="70">
         <v>770.53</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="71">
         <v>1156.5</v>
       </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="109" t="s">
+      <c r="H15" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J15" s="13" t="s">
@@ -1659,8 +1684,8 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="80" customFormat="1">
-      <c r="A16" s="88" t="s">
+    <row r="16" spans="1:11" s="79" customFormat="1">
+      <c r="A16" s="87" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -1669,18 +1694,20 @@
       <c r="C16" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="90">
+      <c r="D16" s="89">
         <v>47300</v>
       </c>
-      <c r="E16" s="71">
+      <c r="E16" s="70">
         <v>240</v>
       </c>
-      <c r="F16" s="72">
+      <c r="F16" s="71">
         <v>360</v>
       </c>
       <c r="G16" s="24"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="109" t="s">
+      <c r="H16" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J16" s="13" t="s">
@@ -1691,8 +1718,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="80" customFormat="1">
-      <c r="A17" s="88" t="s">
+    <row r="17" spans="1:11" s="79" customFormat="1">
+      <c r="A17" s="87" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="16" t="s">
@@ -1701,18 +1728,20 @@
       <c r="C17" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="90">
+      <c r="D17" s="89">
         <v>47300</v>
       </c>
-      <c r="E17" s="71">
+      <c r="E17" s="70">
         <v>1124.0899999999999</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17" s="71">
         <v>1687.5</v>
       </c>
       <c r="G17" s="24"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="109" t="s">
+      <c r="H17" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J17" s="13" t="s">
@@ -1723,31 +1752,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="80" customFormat="1" ht="15" thickBot="1">
-      <c r="A18" s="88" t="s">
+    <row r="18" spans="1:11" s="79" customFormat="1" ht="15" thickBot="1">
+      <c r="A18" s="87" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="89" t="s">
+      <c r="B18" s="88" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="90">
+      <c r="D18" s="89">
         <v>47300</v>
       </c>
-      <c r="E18" s="91">
+      <c r="E18" s="90">
         <v>327.08</v>
       </c>
-      <c r="F18" s="72">
+      <c r="F18" s="71">
         <v>492</v>
       </c>
       <c r="G18" s="24">
         <f>SUM(F14:F18)</f>
         <v>4204.5</v>
       </c>
-      <c r="H18" s="74"/>
-      <c r="I18" s="109" t="s">
+      <c r="H18" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="108" t="s">
         <v>79</v>
       </c>
       <c r="J18" s="13"/>
@@ -1756,19 +1787,19 @@
         <v>10792.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="80" customFormat="1" ht="15" thickTop="1">
-      <c r="A19" s="88"/>
-      <c r="B19" s="89"/>
+    <row r="19" spans="1:11" s="79" customFormat="1" ht="15" thickTop="1">
+      <c r="A19" s="87"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="72"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="71"/>
       <c r="G19" s="24"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="101"/>
-    </row>
-    <row r="20" spans="1:11" s="80" customFormat="1">
-      <c r="A20" s="88" t="s">
+      <c r="H19" s="73"/>
+      <c r="I19" s="100"/>
+    </row>
+    <row r="20" spans="1:11" s="79" customFormat="1">
+      <c r="A20" s="87" t="s">
         <v>71</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1777,133 +1808,141 @@
       <c r="C20" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="90">
+      <c r="D20" s="89">
         <v>47300</v>
       </c>
-      <c r="E20" s="71">
+      <c r="E20" s="70">
         <v>240.92</v>
       </c>
-      <c r="F20" s="72">
+      <c r="F20" s="71">
         <v>361.5</v>
       </c>
       <c r="G20" s="24">
         <f>F20</f>
         <v>361.5</v>
       </c>
-      <c r="H20" s="74"/>
-      <c r="I20" s="109" t="s">
+      <c r="H20" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="108" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="80" customFormat="1">
-      <c r="A21" s="88"/>
+    <row r="21" spans="1:11" s="79" customFormat="1">
+      <c r="A21" s="87"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="72"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="71"/>
       <c r="G21" s="24"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="101"/>
-    </row>
-    <row r="22" spans="1:11" s="80" customFormat="1" ht="79">
-      <c r="A22" s="75" t="s">
+      <c r="H21" s="73"/>
+      <c r="I21" s="100"/>
+    </row>
+    <row r="22" spans="1:11" s="79" customFormat="1" ht="79">
+      <c r="A22" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="70">
+      <c r="D22" s="69">
         <v>44743</v>
       </c>
-      <c r="E22" s="71">
+      <c r="E22" s="70">
         <v>480</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="71">
         <v>960</v>
       </c>
       <c r="G22" s="24"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="110" t="s">
+      <c r="H22" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="109" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="80" customFormat="1" ht="66">
-      <c r="A23" s="75" t="s">
+    <row r="23" spans="1:11" s="79" customFormat="1" ht="66">
+      <c r="A23" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="70">
+      <c r="D23" s="69">
         <v>44743</v>
       </c>
-      <c r="E23" s="71">
+      <c r="E23" s="70">
         <v>160</v>
       </c>
-      <c r="F23" s="72">
+      <c r="F23" s="71">
         <v>320</v>
       </c>
       <c r="G23" s="24">
         <f>SUM(F22:F23)</f>
         <v>1280</v>
       </c>
-      <c r="H23" s="74"/>
-      <c r="I23" s="110" t="s">
+      <c r="H23" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="109" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="80" customFormat="1">
-      <c r="A24" s="75"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="72"/>
+    <row r="24" spans="1:11" s="79" customFormat="1">
+      <c r="A24" s="74"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="71"/>
       <c r="G24" s="24"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="101"/>
-    </row>
-    <row r="25" spans="1:11" s="80" customFormat="1" ht="27">
-      <c r="A25" s="75" t="s">
+      <c r="H24" s="73"/>
+      <c r="I24" s="100"/>
+    </row>
+    <row r="25" spans="1:11" s="79" customFormat="1" ht="27">
+      <c r="A25" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="70">
+      <c r="D25" s="69">
         <v>44743</v>
       </c>
-      <c r="E25" s="71">
+      <c r="E25" s="70">
         <v>20</v>
       </c>
-      <c r="F25" s="72">
+      <c r="F25" s="71">
         <v>40</v>
       </c>
       <c r="G25" s="24">
         <f>F25</f>
         <v>40</v>
       </c>
-      <c r="H25" s="74"/>
-      <c r="I25" s="109" t="s">
+      <c r="H25" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="I25" s="108" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="50" customFormat="1" ht="15" thickBot="1">
-      <c r="A26" s="56"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="58"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="57"/>
       <c r="F26" s="47">
         <f>SUM(F6:F25)</f>
         <v>10792.5</v>
@@ -1913,18 +1952,18 @@
         <v>10752.5</v>
       </c>
       <c r="H26" s="51"/>
-      <c r="I26" s="101"/>
-    </row>
-    <row r="27" spans="1:11" s="59" customFormat="1" ht="15" thickTop="1">
-      <c r="A27" s="76"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="101"/>
+      <c r="I26" s="100"/>
+    </row>
+    <row r="27" spans="1:11" s="58" customFormat="1" ht="15" thickTop="1">
+      <c r="A27" s="75"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="100"/>
     </row>
     <row r="28" spans="1:11" s="15" customFormat="1" ht="15" thickBot="1">
       <c r="A28" s="43"/>
@@ -1935,95 +1974,95 @@
       <c r="F28" s="44"/>
       <c r="G28" s="45"/>
       <c r="H28" s="48"/>
-      <c r="I28" s="101"/>
-    </row>
-    <row r="29" spans="1:11" s="59" customFormat="1" ht="15" thickTop="1">
-      <c r="A29" s="76"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="62"/>
+      <c r="I28" s="100"/>
+    </row>
+    <row r="29" spans="1:11" s="58" customFormat="1" ht="15" thickTop="1">
+      <c r="A29" s="75"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="61"/>
       <c r="G29" s="24"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="101"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="100"/>
     </row>
     <row r="30" spans="1:11" s="12" customFormat="1">
-      <c r="A30" s="76"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="62"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="61"/>
       <c r="G30" s="24"/>
       <c r="H30" s="32"/>
-      <c r="I30" s="101"/>
+      <c r="I30" s="100"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="76"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="62"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="61"/>
       <c r="G31" s="24"/>
       <c r="H31" s="52"/>
-      <c r="I31" s="101"/>
-    </row>
-    <row r="32" spans="1:11" s="59" customFormat="1">
-      <c r="A32" s="76"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="101"/>
+      <c r="I31" s="100"/>
+    </row>
+    <row r="32" spans="1:11" s="58" customFormat="1">
+      <c r="A32" s="75"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="100"/>
     </row>
     <row r="33" spans="1:11" s="12" customFormat="1">
-      <c r="A33" s="76"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="62"/>
+      <c r="A33" s="75"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="61"/>
       <c r="G33" s="24"/>
       <c r="H33" s="11"/>
-      <c r="I33" s="101"/>
-    </row>
-    <row r="34" spans="1:11" s="59" customFormat="1">
-      <c r="A34" s="76"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="62"/>
+      <c r="I33" s="100"/>
+    </row>
+    <row r="34" spans="1:11" s="58" customFormat="1">
+      <c r="A34" s="75"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="61"/>
       <c r="G34" s="24"/>
       <c r="H34" s="11"/>
-      <c r="I34" s="101"/>
+      <c r="I34" s="100"/>
     </row>
     <row r="35" spans="1:11" s="9" customFormat="1">
-      <c r="A35" s="76"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="62"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="24"/>
       <c r="H35" s="11"/>
-      <c r="I35" s="101"/>
+      <c r="I35" s="100"/>
     </row>
     <row r="36" spans="1:11" s="50" customFormat="1">
-      <c r="A36" s="76"/>
-      <c r="B36" s="57"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="62"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="61"/>
       <c r="G36" s="24"/>
       <c r="H36" s="11"/>
-      <c r="I36" s="101"/>
+      <c r="I36" s="100"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="35"/>
@@ -2032,12 +2071,12 @@
       <c r="D37" s="37"/>
       <c r="E37" s="38"/>
       <c r="H37" s="11"/>
-      <c r="I37" s="101"/>
+      <c r="I37" s="100"/>
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="I38" s="101"/>
+      <c r="I38" s="100"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
     </row>
@@ -2050,7 +2089,7 @@
       <c r="F39" s="39"/>
       <c r="G39" s="33"/>
       <c r="H39" s="11"/>
-      <c r="I39" s="101"/>
+      <c r="I39" s="100"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
     </row>
@@ -2063,7 +2102,7 @@
       <c r="F40" s="39"/>
       <c r="G40" s="33"/>
       <c r="H40" s="11"/>
-      <c r="I40" s="101"/>
+      <c r="I40" s="100"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
     </row>
@@ -2076,7 +2115,7 @@
       <c r="F41" s="39"/>
       <c r="G41" s="33"/>
       <c r="H41" s="11"/>
-      <c r="I41" s="101"/>
+      <c r="I41" s="100"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
     </row>
@@ -2089,7 +2128,7 @@
       <c r="F42" s="39"/>
       <c r="G42" s="24"/>
       <c r="H42" s="34"/>
-      <c r="I42" s="101"/>
+      <c r="I42" s="100"/>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
     </row>
@@ -2102,7 +2141,7 @@
       <c r="F43" s="39"/>
       <c r="G43" s="33"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="101"/>
+      <c r="I43" s="100"/>
       <c r="J43" s="16"/>
       <c r="K43" s="16"/>
     </row>
@@ -2115,7 +2154,7 @@
       <c r="F44" s="39"/>
       <c r="G44" s="24"/>
       <c r="H44" s="11"/>
-      <c r="I44" s="101"/>
+      <c r="I44" s="100"/>
       <c r="J44" s="16"/>
     </row>
     <row r="45" spans="1:11" s="9" customFormat="1">
@@ -2127,7 +2166,7 @@
       <c r="F45" s="39"/>
       <c r="G45" s="33"/>
       <c r="H45" s="11"/>
-      <c r="I45" s="101"/>
+      <c r="I45" s="100"/>
       <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:11">
@@ -2139,7 +2178,7 @@
       <c r="F46" s="39"/>
       <c r="G46" s="24"/>
       <c r="H46" s="11"/>
-      <c r="I46" s="101"/>
+      <c r="I46" s="100"/>
       <c r="J46" s="16"/>
     </row>
     <row r="47" spans="1:11">
@@ -2151,7 +2190,7 @@
       <c r="F47" s="39"/>
       <c r="G47" s="33"/>
       <c r="H47" s="11"/>
-      <c r="I47" s="101"/>
+      <c r="I47" s="100"/>
       <c r="J47" s="16"/>
     </row>
     <row r="48" spans="1:11">
@@ -2163,7 +2202,7 @@
       <c r="F48" s="39"/>
       <c r="G48" s="24"/>
       <c r="H48" s="11"/>
-      <c r="I48" s="101"/>
+      <c r="I48" s="100"/>
       <c r="J48" s="16"/>
     </row>
     <row r="49" spans="1:11">
@@ -2175,7 +2214,7 @@
       <c r="F49" s="39"/>
       <c r="G49" s="33"/>
       <c r="H49" s="11"/>
-      <c r="I49" s="101"/>
+      <c r="I49" s="100"/>
       <c r="J49" s="16"/>
     </row>
     <row r="50" spans="1:11" s="9" customFormat="1">
@@ -2187,7 +2226,7 @@
       <c r="F50" s="39"/>
       <c r="G50" s="24"/>
       <c r="H50" s="11"/>
-      <c r="I50" s="101"/>
+      <c r="I50" s="100"/>
       <c r="J50" s="16"/>
     </row>
     <row r="51" spans="1:11">
@@ -2199,7 +2238,7 @@
       <c r="F51" s="39"/>
       <c r="G51" s="24"/>
       <c r="H51" s="11"/>
-      <c r="I51" s="101"/>
+      <c r="I51" s="100"/>
       <c r="J51" s="16"/>
     </row>
     <row r="52" spans="1:11" s="9" customFormat="1">
@@ -2211,7 +2250,7 @@
       <c r="F52" s="39"/>
       <c r="G52" s="24"/>
       <c r="H52" s="34"/>
-      <c r="I52" s="101"/>
+      <c r="I52" s="100"/>
       <c r="J52" s="16"/>
     </row>
     <row r="53" spans="1:11">
@@ -2223,7 +2262,7 @@
       <c r="F53" s="39"/>
       <c r="G53" s="33"/>
       <c r="H53" s="34"/>
-      <c r="I53" s="101"/>
+      <c r="I53" s="100"/>
       <c r="J53" s="16"/>
     </row>
     <row r="54" spans="1:11" s="9" customFormat="1">
@@ -2235,7 +2274,7 @@
       <c r="F54" s="39"/>
       <c r="G54" s="33"/>
       <c r="H54" s="34"/>
-      <c r="I54" s="101"/>
+      <c r="I54" s="100"/>
       <c r="J54" s="16"/>
     </row>
     <row r="55" spans="1:11">
@@ -2247,7 +2286,7 @@
       <c r="F55" s="39"/>
       <c r="G55" s="24"/>
       <c r="H55" s="34"/>
-      <c r="I55" s="101"/>
+      <c r="I55" s="100"/>
       <c r="J55" s="16"/>
     </row>
     <row r="56" spans="1:11" s="9" customFormat="1">
@@ -2259,7 +2298,7 @@
       <c r="F56" s="39"/>
       <c r="G56" s="33"/>
       <c r="H56" s="34"/>
-      <c r="I56" s="101"/>
+      <c r="I56" s="100"/>
       <c r="J56" s="16"/>
       <c r="K56" s="16"/>
     </row>
@@ -2272,7 +2311,7 @@
       <c r="F57" s="39"/>
       <c r="G57" s="24"/>
       <c r="H57" s="34"/>
-      <c r="I57" s="101"/>
+      <c r="I57" s="100"/>
       <c r="J57" s="16"/>
       <c r="K57" s="16"/>
     </row>
@@ -2285,7 +2324,7 @@
       <c r="F58" s="39"/>
       <c r="G58" s="24"/>
       <c r="H58" s="34"/>
-      <c r="I58" s="101"/>
+      <c r="I58" s="100"/>
       <c r="J58" s="16"/>
       <c r="K58" s="16"/>
     </row>
@@ -2298,7 +2337,7 @@
       <c r="F59" s="39"/>
       <c r="G59" s="24"/>
       <c r="H59" s="34"/>
-      <c r="I59" s="101"/>
+      <c r="I59" s="100"/>
       <c r="J59" s="16"/>
       <c r="K59" s="16"/>
     </row>
@@ -2311,7 +2350,7 @@
       <c r="F60" s="39"/>
       <c r="G60" s="34"/>
       <c r="H60" s="34"/>
-      <c r="I60" s="101"/>
+      <c r="I60" s="100"/>
       <c r="J60" s="16"/>
       <c r="K60" s="16"/>
     </row>
@@ -2324,7 +2363,7 @@
       <c r="F61" s="39"/>
       <c r="G61" s="24"/>
       <c r="H61" s="32"/>
-      <c r="I61" s="101"/>
+      <c r="I61" s="100"/>
       <c r="J61" s="16"/>
       <c r="K61" s="16"/>
     </row>
@@ -2337,7 +2376,7 @@
       <c r="F62" s="39"/>
       <c r="G62" s="24"/>
       <c r="H62" s="32"/>
-      <c r="I62" s="101"/>
+      <c r="I62" s="100"/>
       <c r="J62" s="16"/>
       <c r="K62" s="16"/>
     </row>
@@ -2350,7 +2389,7 @@
       <c r="F63" s="39"/>
       <c r="G63" s="24"/>
       <c r="H63" s="32"/>
-      <c r="I63" s="101"/>
+      <c r="I63" s="100"/>
       <c r="J63" s="16"/>
       <c r="K63" s="16"/>
     </row>
@@ -2363,7 +2402,7 @@
       <c r="F64" s="39"/>
       <c r="G64" s="24"/>
       <c r="H64" s="32"/>
-      <c r="I64" s="101"/>
+      <c r="I64" s="100"/>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
     </row>
@@ -2376,7 +2415,7 @@
       <c r="F65" s="39"/>
       <c r="G65" s="24"/>
       <c r="H65" s="32"/>
-      <c r="I65" s="101"/>
+      <c r="I65" s="100"/>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
     </row>
@@ -2389,7 +2428,7 @@
       <c r="F66" s="39"/>
       <c r="G66" s="24"/>
       <c r="H66" s="32"/>
-      <c r="I66" s="101"/>
+      <c r="I66" s="100"/>
       <c r="J66" s="16"/>
       <c r="K66" s="16"/>
     </row>
@@ -2402,7 +2441,7 @@
       <c r="F67" s="39"/>
       <c r="G67" s="24"/>
       <c r="H67" s="32"/>
-      <c r="I67" s="101"/>
+      <c r="I67" s="100"/>
       <c r="J67" s="16"/>
       <c r="K67" s="16"/>
     </row>
@@ -2415,7 +2454,7 @@
       <c r="F68" s="39"/>
       <c r="G68" s="33"/>
       <c r="H68" s="32"/>
-      <c r="I68" s="101"/>
+      <c r="I68" s="100"/>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
     </row>
@@ -2428,7 +2467,7 @@
       <c r="F69" s="39"/>
       <c r="G69" s="24"/>
       <c r="H69" s="32"/>
-      <c r="I69" s="101"/>
+      <c r="I69" s="100"/>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
     </row>
@@ -2441,7 +2480,7 @@
       <c r="F70" s="39"/>
       <c r="G70" s="24"/>
       <c r="H70" s="32"/>
-      <c r="I70" s="101"/>
+      <c r="I70" s="100"/>
       <c r="J70" s="16"/>
       <c r="K70" s="16"/>
     </row>
@@ -2454,7 +2493,7 @@
       <c r="F71" s="39"/>
       <c r="G71" s="24"/>
       <c r="H71" s="32"/>
-      <c r="I71" s="101"/>
+      <c r="I71" s="100"/>
       <c r="J71" s="16"/>
       <c r="K71" s="16"/>
     </row>
@@ -2467,7 +2506,7 @@
       <c r="F72" s="39"/>
       <c r="G72" s="24"/>
       <c r="H72" s="32"/>
-      <c r="I72" s="101"/>
+      <c r="I72" s="100"/>
       <c r="J72" s="16"/>
       <c r="K72" s="16"/>
     </row>
@@ -2480,7 +2519,7 @@
       <c r="F73" s="39"/>
       <c r="G73" s="24"/>
       <c r="H73" s="32"/>
-      <c r="I73" s="101"/>
+      <c r="I73" s="100"/>
       <c r="J73" s="16"/>
       <c r="K73" s="16"/>
     </row>
@@ -2493,7 +2532,7 @@
       <c r="F74" s="39"/>
       <c r="G74" s="33"/>
       <c r="H74" s="32"/>
-      <c r="I74" s="101"/>
+      <c r="I74" s="100"/>
       <c r="J74" s="16"/>
       <c r="K74" s="16"/>
     </row>
@@ -2506,7 +2545,7 @@
       <c r="F75" s="39"/>
       <c r="G75" s="33"/>
       <c r="H75" s="32"/>
-      <c r="I75" s="101"/>
+      <c r="I75" s="100"/>
       <c r="J75" s="16"/>
       <c r="K75" s="16"/>
     </row>
@@ -2519,7 +2558,7 @@
       <c r="F76" s="39"/>
       <c r="G76" s="24"/>
       <c r="H76" s="32"/>
-      <c r="I76" s="101"/>
+      <c r="I76" s="100"/>
       <c r="J76" s="16"/>
       <c r="K76" s="16"/>
     </row>
@@ -2532,7 +2571,7 @@
       <c r="F77" s="39"/>
       <c r="G77" s="24"/>
       <c r="H77" s="32"/>
-      <c r="I77" s="101"/>
+      <c r="I77" s="100"/>
       <c r="J77" s="16"/>
       <c r="K77" s="16"/>
     </row>
@@ -2545,7 +2584,7 @@
       <c r="F78" s="39"/>
       <c r="G78" s="24"/>
       <c r="H78" s="32"/>
-      <c r="I78" s="101"/>
+      <c r="I78" s="100"/>
       <c r="J78" s="16"/>
       <c r="K78" s="16"/>
     </row>
@@ -2558,7 +2597,7 @@
       <c r="F79" s="39"/>
       <c r="G79" s="33"/>
       <c r="H79" s="32"/>
-      <c r="I79" s="101"/>
+      <c r="I79" s="100"/>
       <c r="J79" s="16"/>
       <c r="K79" s="16"/>
     </row>
@@ -2571,7 +2610,7 @@
       <c r="F80" s="39"/>
       <c r="G80" s="33"/>
       <c r="H80" s="32"/>
-      <c r="I80" s="101"/>
+      <c r="I80" s="100"/>
       <c r="J80" s="16"/>
       <c r="K80" s="16"/>
     </row>
@@ -2584,7 +2623,7 @@
       <c r="F81" s="39"/>
       <c r="G81" s="24"/>
       <c r="H81" s="32"/>
-      <c r="I81" s="101"/>
+      <c r="I81" s="100"/>
       <c r="J81" s="16"/>
       <c r="K81" s="16"/>
     </row>
@@ -2597,7 +2636,7 @@
       <c r="F82" s="39"/>
       <c r="G82" s="33"/>
       <c r="H82" s="32"/>
-      <c r="I82" s="101"/>
+      <c r="I82" s="100"/>
       <c r="J82" s="16"/>
       <c r="K82" s="16"/>
     </row>
@@ -2610,7 +2649,7 @@
       <c r="F83" s="39"/>
       <c r="G83" s="24"/>
       <c r="H83" s="32"/>
-      <c r="I83" s="101"/>
+      <c r="I83" s="100"/>
       <c r="J83" s="16"/>
       <c r="K83" s="16"/>
     </row>
@@ -2623,7 +2662,7 @@
       <c r="F84" s="24"/>
       <c r="G84" s="24"/>
       <c r="H84" s="34"/>
-      <c r="I84" s="101"/>
+      <c r="I84" s="100"/>
       <c r="J84" s="16"/>
       <c r="K84" s="16"/>
     </row>
@@ -2636,7 +2675,7 @@
       <c r="F85" s="25"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
-      <c r="I85" s="102"/>
+      <c r="I85" s="101"/>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="25"/>
@@ -2647,7 +2686,7 @@
       <c r="F86" s="25"/>
       <c r="G86" s="25"/>
       <c r="H86" s="25"/>
-      <c r="I86" s="102"/>
+      <c r="I86" s="101"/>
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="25"/>
@@ -2658,7 +2697,7 @@
       <c r="F87" s="25"/>
       <c r="G87" s="25"/>
       <c r="H87" s="25"/>
-      <c r="I87" s="102"/>
+      <c r="I87" s="101"/>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="25"/>
@@ -2669,7 +2708,7 @@
       <c r="F88" s="25"/>
       <c r="G88" s="25"/>
       <c r="H88" s="25"/>
-      <c r="I88" s="102"/>
+      <c r="I88" s="101"/>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="25"/>
@@ -2680,7 +2719,7 @@
       <c r="F89" s="25"/>
       <c r="G89" s="25"/>
       <c r="H89" s="25"/>
-      <c r="I89" s="102"/>
+      <c r="I89" s="101"/>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="25"/>
@@ -2691,7 +2730,7 @@
       <c r="F90" s="25"/>
       <c r="G90" s="25"/>
       <c r="H90" s="25"/>
-      <c r="I90" s="102"/>
+      <c r="I90" s="101"/>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="25"/>
@@ -2702,10 +2741,10 @@
       <c r="F91" s="25"/>
       <c r="G91" s="25"/>
       <c r="H91" s="25"/>
-      <c r="I91" s="102"/>
-    </row>
-    <row r="131" spans="9:9" s="80" customFormat="1">
-      <c r="I131" s="100"/>
+      <c r="I91" s="101"/>
+    </row>
+    <row r="131" spans="9:9" s="79" customFormat="1">
+      <c r="I131" s="99"/>
     </row>
   </sheetData>
   <sortState ref="A6:H25">
@@ -2744,7 +2783,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2756,51 +2795,51 @@
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="30.5" style="100" customWidth="1"/>
+    <col min="8" max="8" width="21.5" style="111" customWidth="1"/>
+    <col min="9" max="9" width="30.5" style="99" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" ht="20">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:11" ht="15">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
@@ -2851,36 +2890,38 @@
       <c r="H5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="100" t="s">
+      <c r="I5" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="99" t="s">
+      <c r="J5" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="99"/>
+      <c r="K5" s="98"/>
     </row>
     <row r="6" spans="1:11" ht="28">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="78" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="79">
+      <c r="C6" s="77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="78">
         <v>44378</v>
       </c>
-      <c r="E6" s="87">
+      <c r="E6" s="86">
         <v>1193.8</v>
       </c>
-      <c r="F6" s="85">
+      <c r="F6" s="84">
         <v>2388</v>
       </c>
       <c r="G6" s="26"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="106" t="s">
+      <c r="H6" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="105" t="s">
         <v>83</v>
       </c>
       <c r="J6" s="30" t="s">
@@ -2892,27 +2933,29 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="28">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="81">
+      <c r="C7" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="80">
         <v>44378</v>
       </c>
-      <c r="E7" s="87">
+      <c r="E7" s="86">
         <v>920</v>
       </c>
-      <c r="F7" s="85">
+      <c r="F7" s="84">
         <v>1840</v>
       </c>
       <c r="G7" s="26"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="106" t="s">
+      <c r="H7" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="105" t="s">
         <v>83</v>
       </c>
       <c r="J7" s="30" t="s">
@@ -2924,652 +2967,704 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="53" customFormat="1" ht="29" thickBot="1">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="81">
+      <c r="C8" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="80">
         <v>44378</v>
       </c>
-      <c r="E8" s="87">
+      <c r="E8" s="86">
         <v>864.95</v>
       </c>
-      <c r="F8" s="85">
+      <c r="F8" s="84">
         <v>1730</v>
       </c>
       <c r="G8" s="26"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="106" t="s">
+      <c r="H8" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="105" t="s">
         <v>83</v>
       </c>
       <c r="J8" s="30"/>
-      <c r="K8" s="55">
+      <c r="K8" s="54">
         <f>SUM(K6:K7)</f>
         <v>21411.5</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="50" customFormat="1" ht="29" thickTop="1">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="81">
+      <c r="C9" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="80">
         <v>44378</v>
       </c>
-      <c r="E9" s="87">
+      <c r="E9" s="86">
         <v>803.9</v>
       </c>
-      <c r="F9" s="85">
+      <c r="F9" s="84">
         <v>1608</v>
       </c>
       <c r="G9" s="26"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="106" t="s">
+      <c r="H9" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="105" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="50" customFormat="1" ht="84">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="78" t="s">
+      <c r="B10" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="81">
+      <c r="C10" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="80">
         <v>44378</v>
       </c>
-      <c r="E10" s="87">
+      <c r="E10" s="86">
         <v>320</v>
       </c>
-      <c r="F10" s="85">
+      <c r="F10" s="84">
         <v>640</v>
       </c>
       <c r="G10" s="26"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="104" t="s">
+      <c r="H10" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" s="103" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="59" customFormat="1" ht="84">
-      <c r="A11" s="77" t="s">
+    <row r="11" spans="1:11" s="58" customFormat="1" ht="84">
+      <c r="A11" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="81">
+      <c r="C11" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="80">
         <v>44378</v>
       </c>
-      <c r="E11" s="87">
+      <c r="E11" s="86">
         <v>318.07</v>
       </c>
-      <c r="F11" s="85">
+      <c r="F11" s="84">
         <v>638</v>
       </c>
       <c r="G11" s="26"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="104" t="s">
+      <c r="H11" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="103" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="59" customFormat="1" ht="28">
-      <c r="A12" s="77" t="s">
+    <row r="12" spans="1:11" s="58" customFormat="1" ht="28">
+      <c r="A12" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="81">
+      <c r="C12" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="80">
         <v>44378</v>
       </c>
-      <c r="E12" s="87">
+      <c r="E12" s="86">
         <v>1600</v>
       </c>
-      <c r="F12" s="85">
+      <c r="F12" s="84">
         <v>3200</v>
       </c>
       <c r="G12" s="27">
         <f>SUM(F6:F12)</f>
         <v>12044</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="105" t="s">
+      <c r="H12" s="110" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="104" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="80" customFormat="1">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="85"/>
+    <row r="13" spans="1:11" s="79" customFormat="1">
+      <c r="A13" s="82"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="84"/>
       <c r="G13" s="27"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="100"/>
-    </row>
-    <row r="14" spans="1:11" s="67" customFormat="1">
-      <c r="A14" s="77" t="s">
+      <c r="H13" s="110"/>
+      <c r="I13" s="99"/>
+    </row>
+    <row r="14" spans="1:11" s="66" customFormat="1">
+      <c r="A14" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="86">
+      <c r="C14" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="85">
         <v>46569</v>
       </c>
-      <c r="E14" s="87">
+      <c r="E14" s="86">
         <v>160</v>
       </c>
-      <c r="F14" s="85">
+      <c r="F14" s="84">
         <v>240</v>
       </c>
       <c r="G14" s="27"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="107" t="s">
+      <c r="H14" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" s="106" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="59" customFormat="1">
-      <c r="A15" s="77" t="s">
+    <row r="15" spans="1:11" s="58" customFormat="1">
+      <c r="A15" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="86">
+      <c r="C15" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="85">
         <v>46569</v>
       </c>
-      <c r="E15" s="87">
+      <c r="E15" s="86">
         <v>120</v>
       </c>
-      <c r="F15" s="85">
+      <c r="F15" s="84">
         <v>180</v>
       </c>
       <c r="G15" s="27"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="107" t="s">
+      <c r="H15" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="106" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="86">
+      <c r="C16" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="85">
         <v>46569</v>
       </c>
-      <c r="E16" s="87">
+      <c r="E16" s="86">
         <v>160</v>
       </c>
-      <c r="F16" s="85">
+      <c r="F16" s="84">
         <v>240</v>
       </c>
-      <c r="H16" s="80"/>
-      <c r="I16" s="107" t="s">
+      <c r="H16" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="106" t="s">
         <v>80</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="86">
+      <c r="C17" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="85">
         <v>46569</v>
       </c>
-      <c r="E17" s="87">
+      <c r="E17" s="86">
         <v>280</v>
       </c>
-      <c r="F17" s="85">
+      <c r="F17" s="84">
         <v>420</v>
       </c>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="107" t="s">
+      <c r="G17" s="79"/>
+      <c r="H17" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" s="106" t="s">
         <v>80</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="78" t="s">
+      <c r="B18" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="86">
+      <c r="C18" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="85">
         <v>46569</v>
       </c>
-      <c r="E18" s="87">
+      <c r="E18" s="86">
         <v>40</v>
       </c>
-      <c r="F18" s="85">
+      <c r="F18" s="84">
         <v>60</v>
       </c>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="107" t="s">
+      <c r="G18" s="79"/>
+      <c r="H18" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="106" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="86">
+      <c r="C19" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="85">
         <v>46569</v>
       </c>
-      <c r="E19" s="87">
+      <c r="E19" s="86">
         <v>200</v>
       </c>
-      <c r="F19" s="85">
+      <c r="F19" s="84">
         <v>300</v>
       </c>
       <c r="G19" s="27">
         <f>SUM(F14:F19)</f>
         <v>1440</v>
       </c>
-      <c r="H19" s="80"/>
-      <c r="I19" s="107" t="s">
+      <c r="H19" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="106" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="80" customFormat="1">
-      <c r="A20" s="83"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="85"/>
-      <c r="I20" s="100"/>
+    <row r="20" spans="1:11" s="79" customFormat="1">
+      <c r="A20" s="82"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="84"/>
+      <c r="H20" s="111"/>
+      <c r="I20" s="99"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="86">
+      <c r="C21" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="85">
         <v>46569</v>
       </c>
-      <c r="E21" s="87">
+      <c r="E21" s="86">
         <v>360</v>
       </c>
-      <c r="F21" s="85">
+      <c r="F21" s="84">
         <v>540</v>
       </c>
       <c r="G21" s="27"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="107" t="s">
+      <c r="H21" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="106" t="s">
         <v>80</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="86">
+      <c r="C22" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="85">
         <v>46569</v>
       </c>
-      <c r="E22" s="87">
+      <c r="E22" s="86">
         <v>240</v>
       </c>
-      <c r="F22" s="85">
+      <c r="F22" s="84">
         <v>360</v>
       </c>
       <c r="G22" s="27"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="107" t="s">
+      <c r="H22" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="106" t="s">
         <v>80</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="78" t="s">
+      <c r="B23" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="86">
+      <c r="C23" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="85">
         <v>46569</v>
       </c>
-      <c r="E23" s="87">
+      <c r="E23" s="86">
         <v>600</v>
       </c>
-      <c r="F23" s="85">
+      <c r="F23" s="84">
         <v>900</v>
       </c>
       <c r="G23" s="27"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="107" t="s">
+      <c r="H23" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="106" t="s">
         <v>80</v>
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="78" t="s">
+      <c r="B24" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="86">
+      <c r="C24" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="85">
         <v>46569</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E24" s="86">
         <v>120</v>
       </c>
-      <c r="F24" s="85">
+      <c r="F24" s="84">
         <v>180</v>
       </c>
       <c r="G24" s="27">
         <f>SUM(F21:F24)</f>
         <v>1980</v>
       </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="107" t="s">
+      <c r="H24" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I24" s="106" t="s">
         <v>80</v>
       </c>
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
     </row>
-    <row r="25" spans="1:11" s="80" customFormat="1">
-      <c r="A25" s="83"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="85"/>
+    <row r="25" spans="1:11" s="79" customFormat="1">
+      <c r="A25" s="82"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="84"/>
       <c r="G25" s="27"/>
-      <c r="I25" s="103"/>
+      <c r="H25" s="111"/>
+      <c r="I25" s="102"/>
     </row>
     <row r="26" spans="1:11" ht="28">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="78" t="s">
+      <c r="B26" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="81">
+      <c r="C26" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="80">
         <v>44378</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="86">
         <v>960</v>
       </c>
-      <c r="F26" s="85">
+      <c r="F26" s="84">
         <v>1920</v>
       </c>
       <c r="G26" s="27"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="108" t="s">
+      <c r="H26" s="111" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" s="107" t="s">
         <v>85</v>
       </c>
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
     </row>
     <row r="27" spans="1:11" ht="28">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="81">
+      <c r="C27" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="80">
         <v>44378</v>
       </c>
-      <c r="E27" s="87">
+      <c r="E27" s="86">
         <v>1049.5999999999999</v>
       </c>
-      <c r="F27" s="85">
+      <c r="F27" s="84">
         <v>2100</v>
       </c>
       <c r="G27" s="27"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="108" t="s">
+      <c r="H27" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I27" s="107" t="s">
         <v>85</v>
       </c>
       <c r="J27" s="17"/>
       <c r="K27" s="17"/>
     </row>
     <row r="28" spans="1:11" ht="56">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="81">
+      <c r="C28" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="80">
         <v>44378</v>
       </c>
-      <c r="E28" s="87">
+      <c r="E28" s="86">
         <v>280.33</v>
       </c>
-      <c r="F28" s="85">
+      <c r="F28" s="84">
         <v>421.5</v>
       </c>
-      <c r="I28" s="106" t="s">
+      <c r="H28" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" s="105" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="56">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="78" t="s">
+      <c r="B29" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="81">
+      <c r="C29" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="80">
         <v>44378</v>
       </c>
-      <c r="E29" s="87">
+      <c r="E29" s="86">
         <v>600</v>
       </c>
-      <c r="F29" s="85">
+      <c r="F29" s="84">
         <v>900</v>
       </c>
       <c r="G29" s="27">
         <f>SUM(F26:F29)</f>
         <v>5341.5</v>
       </c>
-      <c r="I29" s="106" t="s">
+      <c r="H29" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29" s="105" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="80" customFormat="1">
-      <c r="A30" s="83"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="85"/>
-      <c r="I30" s="100"/>
+    <row r="30" spans="1:11" s="79" customFormat="1">
+      <c r="A30" s="82"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="84"/>
+      <c r="H30" s="111"/>
+      <c r="I30" s="99"/>
     </row>
     <row r="31" spans="1:11" ht="42">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="78" t="s">
+      <c r="B31" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="81">
+      <c r="C31" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="80">
         <v>44378</v>
       </c>
-      <c r="E31" s="87">
+      <c r="E31" s="86">
         <v>10.32</v>
       </c>
-      <c r="F31" s="85">
+      <c r="F31" s="84">
         <v>22</v>
       </c>
       <c r="G31" s="26"/>
-      <c r="H31" s="82"/>
-      <c r="I31" s="106" t="s">
+      <c r="H31" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I31" s="105" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="56">
-      <c r="A32" s="77" t="s">
+      <c r="A32" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="78" t="s">
+      <c r="B32" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="81">
+      <c r="C32" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="80">
         <v>44378</v>
       </c>
-      <c r="E32" s="87">
+      <c r="E32" s="86">
         <v>5.88</v>
       </c>
-      <c r="F32" s="85">
+      <c r="F32" s="84">
         <v>12</v>
       </c>
       <c r="G32" s="26"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="106" t="s">
+      <c r="H32" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" s="105" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="28">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="81">
+      <c r="C33" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="80">
         <v>44378</v>
       </c>
-      <c r="E33" s="87">
+      <c r="E33" s="86">
         <v>40</v>
       </c>
-      <c r="F33" s="85">
+      <c r="F33" s="84">
         <v>80</v>
       </c>
       <c r="G33" s="26"/>
-      <c r="H33" s="82"/>
-      <c r="I33" s="106" t="s">
+      <c r="H33" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" s="105" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="70">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="81">
+      <c r="C34" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="80">
         <v>44378</v>
       </c>
-      <c r="E34" s="87">
+      <c r="E34" s="86">
         <v>245.38</v>
       </c>
-      <c r="F34" s="85">
+      <c r="F34" s="84">
         <v>492</v>
       </c>
       <c r="G34" s="27">
         <f>SUM(F31:F34)</f>
         <v>606</v>
       </c>
-      <c r="I34" s="105" t="s">
+      <c r="H34" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="I34" s="104" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1">
-      <c r="A35" s="69"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
       <c r="D35" s="28"/>
@@ -3582,7 +3677,7 @@
         <f>SUM(G6:G34)</f>
         <v>21411.5</v>
       </c>
-      <c r="H35" s="28"/>
+      <c r="H35" s="112"/>
     </row>
     <row r="36" spans="1:9" ht="15" thickTop="1"/>
   </sheetData>

</xml_diff>